<commit_message>
changes in the reset page
</commit_message>
<xml_diff>
--- a/src/main/resources/datamanagement/Testdata.xlsx
+++ b/src/main/resources/datamanagement/Testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muham\IdeaProjects\qalegend\src\main\resources\datamanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44E1A0B-EFA0-43A8-B475-AF5E06AC2598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CD3CA8-16BC-42B4-83E9-0723C0E7AB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
+    <sheet name="ResetPage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>expectedtitle</t>
   </si>
@@ -49,6 +50,12 @@
   </si>
   <si>
     <t>anas</t>
+  </si>
+  <si>
+    <t>expectedmessage</t>
+  </si>
+  <si>
+    <t>We can't find a user with that e-mail address.</t>
   </si>
 </sst>
 </file>
@@ -386,7 +393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -434,4 +441,31 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE09DFA-E772-4B1D-B623-CFCC093B80E7}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add category functionality
- Implement category addition  with validation using faker
-
</commit_message>
<xml_diff>
--- a/src/main/resources/datamanagement/Testdata.xlsx
+++ b/src/main/resources/datamanagement/Testdata.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muham\IdeaProjects\qalegend\src\main\resources\datamanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF33F324-5CCF-4CE3-9F6D-4DB14442A02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D19E1C-8D51-4280-B6E1-20EFC3605128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3144" yWindow="3228" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
-    <sheet name="ManageUsers" sheetId="4" r:id="rId2"/>
-    <sheet name="ResetPage" sheetId="2" r:id="rId3"/>
-    <sheet name="UserManagement" sheetId="3" r:id="rId4"/>
+    <sheet name="Products" sheetId="5" r:id="rId2"/>
+    <sheet name="ManageUsers" sheetId="4" r:id="rId3"/>
+    <sheet name="ResetPage" sheetId="2" r:id="rId4"/>
+    <sheet name="UserManagement" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>expectedtitle</t>
   </si>
@@ -76,6 +77,18 @@
   </si>
   <si>
     <t>Anas</t>
+  </si>
+  <si>
+    <t>Variations;Import Products;Import Opening Stock;Selling Price Group;Units;Categories ;Brands</t>
+  </si>
+  <si>
+    <t>categoryName</t>
+  </si>
+  <si>
+    <t>Tea powder</t>
+  </si>
+  <si>
+    <t>categoryCode</t>
   </si>
 </sst>
 </file>
@@ -126,11 +139,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -414,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -473,6 +489,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739BE882-79DD-47D2-9979-F056F9A38A9A}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="78.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDB0FAF-62E8-48C0-AD6F-A442ECDF5B33}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -499,7 +558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE09DFA-E772-4B1D-B623-CFCC093B80E7}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -526,7 +585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C7EC3A-5B6D-4041-9173-8F049003837C}">
   <dimension ref="A1:B1"/>
   <sheetViews>

</xml_diff>